<commit_message>
[fix] - complete change require from last meeting
</commit_message>
<xml_diff>
--- a/MANAGER/Excel_template/TemplateKinhPhiDuTru.xlsx
+++ b/MANAGER/Excel_template/TemplateKinhPhiDuTru.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shido\Desktop\Science-Management-and-International-Affairs\MANAGER\Excel_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1203DEFA-1CF2-4DEA-9674-D3AF91B08163}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F893A8-5D31-4975-8691-38CDDB7484DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{98BBD7A4-4697-47E2-8457-1602E662089E}"/>
   </bookViews>
@@ -110,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -118,6 +118,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,16 +436,18 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="27.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>